<commit_message>
fix to migration 15
</commit_message>
<xml_diff>
--- a/migration_data/SituationalDashboard.xlsx
+++ b/migration_data/SituationalDashboard.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19840" windowHeight="16420" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="19840" windowHeight="16420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="chart_index" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,315 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="167">
   <si>
+    <t># children missed due to refusal - PCA</t>
+  </si>
+  <si>
+    <t># children missed due to not available - PCA</t>
+  </si>
+  <si>
+    <t># children missed due to no team visit - PCA</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of Environmental Samples collected</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of Adequate Specimen </t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of Environmental Samples with Negative result</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent Missed Children - Out of House Survey</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent Missed Children - Out of House Survey</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent Missed Children - PCA</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Immunity Profile</t>
+  </si>
+  <si>
+    <t>100% Stacked Bar</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>t4</t>
+  </si>
+  <si>
+    <t>Non Polio AFP Rate &amp; Adequate Specimens</t>
+  </si>
+  <si>
+    <t>Bar / Line</t>
+  </si>
+  <si>
+    <t>t5</t>
+  </si>
+  <si>
+    <t>Innaccessable Children</t>
+  </si>
+  <si>
+    <t>Bar</t>
+  </si>
+  <si>
+    <t>campaign</t>
+  </si>
+  <si>
+    <t>t6</t>
+  </si>
+  <si>
+    <t>Environmental Results</t>
+  </si>
+  <si>
+    <t>100% Stacked bar</t>
+  </si>
+  <si>
+    <t>t7</t>
+  </si>
+  <si>
+    <t>t8</t>
+  </si>
+  <si>
+    <t>Campaign Analysis</t>
+  </si>
+  <si>
+    <t>t9</t>
+  </si>
+  <si>
+    <t>Campaign Analysis - Pie Chart</t>
+  </si>
+  <si>
+    <t>Pie Chart</t>
+  </si>
+  <si>
+    <t>t10</t>
+  </si>
+  <si>
+    <t>Missed Children Trend</t>
+  </si>
+  <si>
+    <t>Grouped Bar</t>
+  </si>
+  <si>
+    <t>t11</t>
+  </si>
+  <si>
+    <t>Number Inaccessible Children</t>
+  </si>
+  <si>
+    <t>Total target children</t>
+  </si>
+  <si>
+    <t>Last polio case</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of Environmental Samples collected</t>
+  </si>
+  <si>
+    <t>Missed Chilren By Reason</t>
+  </si>
+  <si>
+    <t>Stacked and Grouped Bar</t>
+  </si>
+  <si>
+    <t>t12</t>
+  </si>
+  <si>
+    <t>LQAS</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Number of reported Non Polio AFP cases</t>
+  </si>
+  <si>
+    <t>Number of Unvaccinated Non Polio AFP Cases</t>
+  </si>
+  <si>
+    <t>Number of Non Polio AFP cases vaccinated 1-3 doses</t>
+  </si>
+  <si>
+    <t>Number of Non Polio AFP cases vaccinated 4-6 doses</t>
+  </si>
+  <si>
+    <t>Number of Non Polio AFP cases vaccinated 7+ doses</t>
+  </si>
+  <si>
+    <t>Non Polio AFP Rate</t>
+  </si>
+  <si>
+    <t>SIA service providers identified</t>
+  </si>
+  <si>
+    <t>Percent FLW_operation paid</t>
+  </si>
+  <si>
+    <t>Missed Children PCA vs. Out Of House</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of children missed due to all access issues</t>
+  </si>
+  <si>
+    <t>District</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>District</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent FLW_social mobilisers paid</t>
+  </si>
+  <si>
+    <t>Percent volunteers attended training sessions</t>
+  </si>
+  <si>
+    <t>Number of Environmental Samples with Negative result</t>
+  </si>
+  <si>
+    <t>Number of Environmental Samples with Positive result</t>
+  </si>
+  <si>
+    <t>Number of Environmental Samples with result pending in Lab</t>
+  </si>
+  <si>
+    <t>Supervision and monitoring plan</t>
+  </si>
+  <si>
+    <t>Social mobilization plan</t>
+  </si>
+  <si>
+    <t>District Governor multi-sectoral meeting on Polio</t>
+  </si>
+  <si>
+    <t>Number.Vaccinated.Recorded.3days</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>fake</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number.Children.withFM.Market.Survey</t>
+  </si>
+  <si>
+    <t># children seen - PCA</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t7</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Target.Population</t>
+  </si>
+  <si>
+    <t>Number.Missed.Recorded.3days</t>
+  </si>
+  <si>
+    <t>Number.Recovered.3days</t>
+  </si>
+  <si>
+    <t>Percent.Vaccinated.Recorded.3days</t>
+  </si>
+  <si>
+    <t>Percent.Missed.Recorded.3days</t>
+  </si>
+  <si>
+    <t>Number.Recovered.5thDay</t>
+  </si>
+  <si>
+    <t>Total.Recovered</t>
+  </si>
+  <si>
+    <t>Number.Missed.Remain</t>
+  </si>
+  <si>
+    <t>Percent.Missed.Remain</t>
+  </si>
+  <si>
+    <t>Percent.Vaccinated.5days</t>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t8</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent of FLWs (social mobilisers) paid last campaign</t>
+  </si>
+  <si>
+    <t>Percent FLWs (operation) paid</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percent FLWs (operation) paid last campaign</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number.Children.Seen.Market.Survey</t>
+  </si>
+  <si>
+    <t>Percent.Coverage.Market.Survey</t>
+  </si>
+  <si>
+    <t>Number.Children.withFM.PCA</t>
+  </si>
+  <si>
+    <t>Number.Children.SeenPCA</t>
+  </si>
+  <si>
+    <t>Percent.Coverage.PCA</t>
+  </si>
+  <si>
+    <t>t9</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>t10</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t># children seen - PCA</t>
+  </si>
+  <si>
     <t>Supervision and Monitoring Plan</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
@@ -265,315 +574,6 @@
   </si>
   <si>
     <t>t6</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of Environmental Samples collected</t>
-  </si>
-  <si>
-    <t>Missed Chilren By Reason</t>
-  </si>
-  <si>
-    <t>Stacked and Grouped Bar</t>
-  </si>
-  <si>
-    <t>t12</t>
-  </si>
-  <si>
-    <t>LQAS</t>
-  </si>
-  <si>
-    <t>Province</t>
-  </si>
-  <si>
-    <t>District</t>
-  </si>
-  <si>
-    <t>Number of reported Non Polio AFP cases</t>
-  </si>
-  <si>
-    <t>Number of Unvaccinated Non Polio AFP Cases</t>
-  </si>
-  <si>
-    <t>Number of Non Polio AFP cases vaccinated 1-3 doses</t>
-  </si>
-  <si>
-    <t>Number of Non Polio AFP cases vaccinated 4-6 doses</t>
-  </si>
-  <si>
-    <t>Number of Non Polio AFP cases vaccinated 7+ doses</t>
-  </si>
-  <si>
-    <t>Non Polio AFP Rate</t>
-  </si>
-  <si>
-    <t>SIA service providers identified</t>
-  </si>
-  <si>
-    <t>Percent FLW_operation paid</t>
-  </si>
-  <si>
-    <t>Missed Children PCA vs. Out Of House</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t2</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t2</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of children missed due to all access issues</t>
-  </si>
-  <si>
-    <t>District</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>District</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent FLW_social mobilisers paid</t>
-  </si>
-  <si>
-    <t>Percent volunteers attended training sessions</t>
-  </si>
-  <si>
-    <t>Number of Environmental Samples with Negative result</t>
-  </si>
-  <si>
-    <t>Number of Environmental Samples with Positive result</t>
-  </si>
-  <si>
-    <t>Number of Environmental Samples with result pending in Lab</t>
-  </si>
-  <si>
-    <t>Supervision and monitoring plan</t>
-  </si>
-  <si>
-    <t>Social mobilization plan</t>
-  </si>
-  <si>
-    <t>District Governor multi-sectoral meeting on Polio</t>
-  </si>
-  <si>
-    <t>Number.Vaccinated.Recorded.3days</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>fake</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number.Children.withFM.Market.Survey</t>
-  </si>
-  <si>
-    <t># children seen - PCA</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t7</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Target.Population</t>
-  </si>
-  <si>
-    <t>Number.Missed.Recorded.3days</t>
-  </si>
-  <si>
-    <t>Number.Recovered.3days</t>
-  </si>
-  <si>
-    <t>Percent.Vaccinated.Recorded.3days</t>
-  </si>
-  <si>
-    <t>Percent.Missed.Recorded.3days</t>
-  </si>
-  <si>
-    <t>Number.Recovered.5thDay</t>
-  </si>
-  <si>
-    <t>Total.Recovered</t>
-  </si>
-  <si>
-    <t>Number.Missed.Remain</t>
-  </si>
-  <si>
-    <t>Percent.Missed.Remain</t>
-  </si>
-  <si>
-    <t>Percent.Vaccinated.5days</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t8</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent of FLWs (social mobilisers) paid last campaign</t>
-  </si>
-  <si>
-    <t>Percent FLWs (operation) paid</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent FLWs (operation) paid last campaign</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number.Children.Seen.Market.Survey</t>
-  </si>
-  <si>
-    <t>Percent.Coverage.Market.Survey</t>
-  </si>
-  <si>
-    <t>Number.Children.withFM.PCA</t>
-  </si>
-  <si>
-    <t>Number.Children.SeenPCA</t>
-  </si>
-  <si>
-    <t>Percent.Coverage.PCA</t>
-  </si>
-  <si>
-    <t>t9</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>t10</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t># children seen - PCA</t>
-  </si>
-  <si>
-    <t># children missed due to refusal - PCA</t>
-  </si>
-  <si>
-    <t># children missed due to not available - PCA</t>
-  </si>
-  <si>
-    <t># children missed due to no team visit - PCA</t>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of Environmental Samples collected</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage of Adequate Specimen </t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of Environmental Samples with Negative result</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent Missed Children - Out of House Survey</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent Missed Children - Out of House Survey</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percent Missed Children - PCA</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>Immunity Profile</t>
-  </si>
-  <si>
-    <t>100% Stacked Bar</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>t4</t>
-  </si>
-  <si>
-    <t>Non Polio AFP Rate &amp; Adequate Specimens</t>
-  </si>
-  <si>
-    <t>Bar / Line</t>
-  </si>
-  <si>
-    <t>t5</t>
-  </si>
-  <si>
-    <t>Innaccessable Children</t>
-  </si>
-  <si>
-    <t>Bar</t>
-  </si>
-  <si>
-    <t>campaign</t>
-  </si>
-  <si>
-    <t>t6</t>
-  </si>
-  <si>
-    <t>Environmental Results</t>
-  </si>
-  <si>
-    <t>100% Stacked bar</t>
-  </si>
-  <si>
-    <t>t7</t>
-  </si>
-  <si>
-    <t>t8</t>
-  </si>
-  <si>
-    <t>Campaign Analysis</t>
-  </si>
-  <si>
-    <t>t9</t>
-  </si>
-  <si>
-    <t>Campaign Analysis - Pie Chart</t>
-  </si>
-  <si>
-    <t>Pie Chart</t>
-  </si>
-  <si>
-    <t>t10</t>
-  </si>
-  <si>
-    <t>Missed Children Trend</t>
-  </si>
-  <si>
-    <t>Grouped Bar</t>
-  </si>
-  <si>
-    <t>t11</t>
-  </si>
-  <si>
-    <t>Number Inaccessible Children</t>
-  </si>
-  <si>
-    <t>Total target children</t>
-  </si>
-  <si>
-    <t>Last polio case</t>
-  </si>
-  <si>
-    <t>int</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -953,7 +953,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -964,8 +964,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.5" defaultRowHeight="15" customHeight="1"/>
@@ -978,62 +978,62 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>156</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>160</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>139</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>159</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>53</v>
+        <v>148</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>46</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>143</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>144</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>147</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="G3" s="1">
         <v>28</v>
@@ -1041,22 +1041,22 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>122</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="G4" s="1">
         <v>28</v>
@@ -1064,22 +1064,22 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>140</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>141</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1">
         <v>28</v>
@@ -1087,22 +1087,22 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>143</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>145</v>
+        <v>16</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="G6" s="1">
         <v>16</v>
@@ -1110,22 +1110,22 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>147</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>148</v>
+        <v>19</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>149</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1">
         <v>3</v>
@@ -1133,22 +1133,22 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>150</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>152</v>
+        <v>23</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>50</v>
+        <v>145</v>
       </c>
       <c r="G8" s="1">
         <v>28</v>
@@ -1156,22 +1156,22 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="1" t="s">
-        <v>153</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>106</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>149</v>
+        <v>20</v>
       </c>
       <c r="G9" s="1">
         <v>3</v>
@@ -1179,22 +1179,22 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="1" t="s">
-        <v>154</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>155</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>149</v>
+        <v>20</v>
       </c>
       <c r="G10" s="1">
         <v>3</v>
@@ -1202,22 +1202,22 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>156</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>157</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>158</v>
+        <v>29</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>149</v>
+        <v>20</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -1225,22 +1225,22 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="1" t="s">
-        <v>159</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>160</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>161</v>
+        <v>32</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>149</v>
+        <v>20</v>
       </c>
       <c r="G12" s="1">
         <v>3</v>
@@ -1248,22 +1248,22 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="1" t="s">
-        <v>162</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>78</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>149</v>
+        <v>20</v>
       </c>
       <c r="G13" s="1">
         <v>3</v>
@@ -1271,22 +1271,22 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="1" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="E14" s="1">
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>149</v>
+        <v>20</v>
       </c>
       <c r="G14" s="1">
         <v>3</v>
@@ -1294,22 +1294,22 @@
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>4</v>
+        <v>99</v>
       </c>
       <c r="E15" s="1">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="G15" s="1">
         <v>28</v>
@@ -1331,7 +1331,7 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -1352,28 +1352,28 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>149</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>57</v>
+        <v>152</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>58</v>
+        <v>153</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>59</v>
+        <v>154</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>60</v>
+        <v>155</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>61</v>
+        <v>156</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1381,16 +1381,16 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>164</v>
+        <v>35</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>164</v>
+        <v>35</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>164</v>
+        <v>35</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>166</v>
+        <v>37</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -1399,10 +1399,10 @@
         <v>0</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>40</v>
+        <v>135</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -1410,16 +1410,16 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>165</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>165</v>
+        <v>36</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>165</v>
+        <v>36</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -1428,10 +1428,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>40</v>
+        <v>135</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -1440,16 +1440,16 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E4" s="5">
         <v>1</v>
@@ -1458,10 +1458,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -1470,16 +1470,16 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>42</v>
+        <v>137</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>42</v>
+        <v>137</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>42</v>
+        <v>137</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E5" s="5">
         <v>1</v>
@@ -1488,10 +1488,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1500,16 +1500,16 @@
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>43</v>
+        <v>138</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E6" s="5">
         <v>1</v>
@@ -1518,10 +1518,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -1530,16 +1530,16 @@
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>63</v>
+        <v>158</v>
       </c>
       <c r="E7" s="4">
         <v>1</v>
@@ -1548,10 +1548,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1560,16 +1560,16 @@
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>63</v>
+        <v>158</v>
       </c>
       <c r="E8" s="4">
         <v>1</v>
@@ -1578,10 +1578,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1590,16 +1590,16 @@
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>63</v>
+        <v>158</v>
       </c>
       <c r="E9" s="4">
         <v>1</v>
@@ -1608,10 +1608,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1620,16 +1620,16 @@
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>63</v>
+        <v>158</v>
       </c>
       <c r="E10" s="4">
         <v>1</v>
@@ -1638,10 +1638,10 @@
         <v>0</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1650,16 +1650,16 @@
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>63</v>
+        <v>158</v>
       </c>
       <c r="E11" s="4">
         <v>1</v>
@@ -1668,10 +1668,10 @@
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1680,16 +1680,16 @@
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>163</v>
+        <v>34</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>163</v>
+        <v>34</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>63</v>
+        <v>158</v>
       </c>
       <c r="E12" s="4">
         <v>1</v>
@@ -1698,10 +1698,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1710,16 +1710,16 @@
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E13" s="10">
         <v>1</v>
@@ -1728,10 +1728,10 @@
         <v>0</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>62</v>
+        <v>157</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>143</v>
+        <v>14</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1740,16 +1740,16 @@
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>135</v>
+        <v>6</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>69</v>
+        <v>164</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>69</v>
+        <v>164</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
@@ -1758,10 +1758,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>70</v>
+        <v>165</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>68</v>
+        <v>163</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1770,16 +1770,16 @@
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1">
       <c r="A15" s="11" t="s">
-        <v>134</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E15" s="5">
         <v>1</v>
@@ -1788,10 +1788,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>71</v>
+        <v>166</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1800,16 +1800,16 @@
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1">
       <c r="A16" s="11" t="s">
-        <v>136</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E16" s="5">
         <v>1</v>
@@ -1818,10 +1818,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>71</v>
+        <v>166</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1830,16 +1830,16 @@
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E17" s="5">
         <v>1</v>
@@ -1848,10 +1848,10 @@
         <v>0</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>71</v>
+        <v>166</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1860,16 +1860,16 @@
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E18" s="5">
         <v>1</v>
@@ -1878,10 +1878,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>71</v>
+        <v>166</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1890,16 +1890,16 @@
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E19" s="5">
         <v>1</v>
@@ -1908,10 +1908,10 @@
         <v>0</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1920,16 +1920,16 @@
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1">
       <c r="A20" s="11" t="s">
-        <v>31</v>
+        <v>126</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>31</v>
+        <v>126</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>32</v>
+        <v>127</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E20" s="5">
         <v>1</v>
@@ -1938,10 +1938,10 @@
         <v>0</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1950,16 +1950,16 @@
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>34</v>
+        <v>129</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>34</v>
+        <v>129</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>34</v>
+        <v>129</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>
@@ -1968,10 +1968,10 @@
         <v>0</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -1980,16 +1980,16 @@
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
@@ -1998,10 +1998,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -2010,16 +2010,16 @@
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>38</v>
+        <v>133</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>38</v>
+        <v>133</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E23" s="5">
         <v>1</v>
@@ -2028,10 +2028,10 @@
         <v>0</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -2040,16 +2040,16 @@
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E24" s="5">
         <v>1</v>
@@ -2058,10 +2058,10 @@
         <v>0</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2070,16 +2070,16 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>37</v>
+        <v>132</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
@@ -2088,10 +2088,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2100,16 +2100,16 @@
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E26" s="5">
         <v>1</v>
@@ -2118,10 +2118,10 @@
         <v>0</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -2130,16 +2130,16 @@
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>118</v>
+        <v>84</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E27" s="5">
         <v>1</v>
@@ -2148,10 +2148,10 @@
         <v>0</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -2160,16 +2160,16 @@
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E28" s="5">
         <v>1</v>
@@ -2178,10 +2178,10 @@
         <v>0</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -2190,16 +2190,16 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>133</v>
+        <v>4</v>
       </c>
       <c r="E29" s="5">
         <v>1</v>
@@ -2208,10 +2208,10 @@
         <v>0</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -2220,16 +2220,16 @@
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>35</v>
+        <v>130</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>35</v>
+        <v>130</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>35</v>
+        <v>130</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>166</v>
+        <v>37</v>
       </c>
       <c r="E30" s="5">
         <v>1</v>
@@ -2238,10 +2238,10 @@
         <v>0</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
@@ -2250,16 +2250,16 @@
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>106</v>
+        <v>72</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="E31" s="5">
         <v>1</v>
@@ -2268,10 +2268,10 @@
         <v>0</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
@@ -2280,16 +2280,16 @@
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="E32" s="5">
         <v>1</v>
@@ -2298,10 +2298,10 @@
         <v>0</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
@@ -2310,16 +2310,16 @@
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E33" s="5">
         <v>1</v>
@@ -2328,10 +2328,10 @@
         <v>0</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -2340,16 +2340,16 @@
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E34" s="5">
         <v>1</v>
@@ -2358,10 +2358,10 @@
         <v>0</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -2370,16 +2370,16 @@
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E35" s="5">
         <v>1</v>
@@ -2388,10 +2388,10 @@
         <v>0</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -2400,16 +2400,16 @@
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E36" s="5">
         <v>1</v>
@@ -2418,10 +2418,10 @@
         <v>0</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -2430,16 +2430,16 @@
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E37" s="5">
         <v>1</v>
@@ -2448,10 +2448,10 @@
         <v>0</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -2460,16 +2460,16 @@
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E38" s="5">
         <v>1</v>
@@ -2478,10 +2478,10 @@
         <v>0</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -2490,16 +2490,16 @@
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E39" s="5">
         <v>1</v>
@@ -2508,10 +2508,10 @@
         <v>0</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -2520,16 +2520,16 @@
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>166</v>
+        <v>37</v>
       </c>
       <c r="E40" s="5">
         <v>1</v>
@@ -2538,10 +2538,10 @@
         <v>0</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>67</v>
+        <v>162</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
@@ -2550,16 +2550,16 @@
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E41" s="5">
         <v>1</v>
@@ -2568,10 +2568,10 @@
         <v>0</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2"/>
@@ -2580,16 +2580,16 @@
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E42" s="5">
         <v>1</v>
@@ -2598,10 +2598,10 @@
         <v>0</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -2610,16 +2610,16 @@
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E43" s="5">
         <v>1</v>
@@ -2628,10 +2628,10 @@
         <v>0</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
@@ -2640,16 +2640,16 @@
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E44" s="5">
         <v>1</v>
@@ -2658,10 +2658,10 @@
         <v>0</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
@@ -2670,16 +2670,16 @@
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1">
       <c r="A45" s="8" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>122</v>
+        <v>88</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E45" s="5">
         <v>1</v>
@@ -2688,10 +2688,10 @@
         <v>0</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -2700,16 +2700,16 @@
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>123</v>
+        <v>89</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E46" s="5">
         <v>1</v>
@@ -2718,10 +2718,10 @@
         <v>0</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -2730,16 +2730,16 @@
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1">
       <c r="A47" s="8" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E47" s="5">
         <v>1</v>
@@ -2748,10 +2748,10 @@
         <v>0</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -2760,16 +2760,16 @@
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E48" s="5">
         <v>1</v>
@@ -2778,10 +2778,10 @@
         <v>0</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -2790,16 +2790,16 @@
     </row>
     <row r="49" spans="1:12" ht="15.75" customHeight="1">
       <c r="A49" s="8" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E49" s="5">
         <v>1</v>
@@ -2808,10 +2808,10 @@
         <v>0</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -2820,16 +2820,16 @@
     </row>
     <row r="50" spans="1:12" ht="15.75" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>166</v>
+        <v>37</v>
       </c>
       <c r="E50" s="5">
         <v>1</v>
@@ -2838,10 +2838,10 @@
         <v>0</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -2850,16 +2850,16 @@
     </row>
     <row r="51" spans="1:12" ht="15.75" customHeight="1">
       <c r="A51" s="8" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>114</v>
+        <v>80</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E51" s="5">
         <v>1</v>
@@ -2868,10 +2868,10 @@
         <v>0</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -2880,16 +2880,16 @@
     </row>
     <row r="52" spans="1:12" ht="15.75" customHeight="1">
       <c r="A52" s="9" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E52" s="5">
         <v>1</v>
@@ -2898,10 +2898,10 @@
         <v>0</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -2910,16 +2910,16 @@
     </row>
     <row r="53" spans="1:12" ht="15.75" customHeight="1">
       <c r="A53" s="9" t="s">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E53" s="5">
         <v>1</v>
@@ -2928,10 +2928,10 @@
         <v>0</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -2940,16 +2940,16 @@
     </row>
     <row r="54" spans="1:12" ht="15.75" customHeight="1">
       <c r="A54" s="9" t="s">
-        <v>130</v>
+        <v>1</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>130</v>
+        <v>1</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>130</v>
+        <v>1</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E54" s="5">
         <v>1</v>
@@ -2958,10 +2958,10 @@
         <v>0</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -2970,16 +2970,16 @@
     </row>
     <row r="55" spans="1:12" ht="15.75" customHeight="1">
       <c r="A55" s="9" t="s">
-        <v>131</v>
+        <v>2</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>131</v>
+        <v>2</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>131</v>
+        <v>2</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E55" s="5">
         <v>1</v>
@@ -2988,10 +2988,10 @@
         <v>0</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -3000,16 +3000,16 @@
     </row>
     <row r="56" spans="1:12" ht="15.75" customHeight="1">
       <c r="A56" s="9" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E56" s="5">
         <v>1</v>
@@ -3018,10 +3018,10 @@
         <v>0</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -3030,16 +3030,16 @@
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1">
       <c r="A57" s="9" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E57" s="5">
         <v>1</v>
@@ -3048,10 +3048,10 @@
         <v>0</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
@@ -3060,16 +3060,16 @@
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1">
       <c r="A58" s="9" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E58" s="5">
         <v>1</v>
@@ -3078,10 +3078,10 @@
         <v>0</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
@@ -3090,16 +3090,16 @@
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1">
       <c r="A59" s="9" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E59" s="5">
         <v>1</v>
@@ -3108,10 +3108,10 @@
         <v>0</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -3120,16 +3120,16 @@
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1">
       <c r="A60" s="9" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E60" s="5">
         <v>1</v>
@@ -3138,10 +3138,10 @@
         <v>0</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>18</v>
+        <v>113</v>
       </c>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
@@ -3150,16 +3150,16 @@
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1">
       <c r="A61" s="8" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E61" s="5">
         <v>1</v>
@@ -3168,10 +3168,10 @@
         <v>0</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -3180,16 +3180,16 @@
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1">
       <c r="A62" s="8" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>20</v>
+        <v>115</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E62" s="5">
         <v>1</v>
@@ -3198,10 +3198,10 @@
         <v>0</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
@@ -3210,16 +3210,16 @@
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1">
       <c r="A63" s="8" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="E63" s="5">
         <v>1</v>
@@ -3228,10 +3228,10 @@
         <v>0</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
@@ -3240,16 +3240,16 @@
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1">
       <c r="A64" s="5" t="s">
-        <v>137</v>
+        <v>8</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>6</v>
+        <v>101</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E64" s="5">
         <v>1</v>
@@ -3258,10 +3258,10 @@
         <v>0</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
@@ -3270,16 +3270,16 @@
     </row>
     <row r="65" spans="1:12" ht="15.75" customHeight="1">
       <c r="A65" s="5" t="s">
-        <v>139</v>
+        <v>10</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>139</v>
+        <v>10</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="E65" s="5">
         <v>1</v>
@@ -3288,10 +3288,10 @@
         <v>0</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="H65" s="5" t="s">
-        <v>1</v>
+        <v>96</v>
       </c>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
@@ -3300,16 +3300,16 @@
     </row>
     <row r="66" spans="1:12" ht="15.75" customHeight="1">
       <c r="A66" s="5" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>9</v>
+        <v>104</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="E66" s="5">
         <v>1</v>
@@ -3318,10 +3318,10 @@
         <v>0</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
@@ -11837,7 +11837,6 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>